<commit_message>
run through sample files, fix excel inputs
</commit_message>
<xml_diff>
--- a/SampleInputs/Contacts-Sample-crosscountry.xlsx
+++ b/SampleInputs/Contacts-Sample-crosscountry.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/DistributedBirding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/DistributedBirding/SampleInputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E0033-64A6-9A45-A27E-B3D2365B6263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE12B28B-40E8-3742-A500-EC2DD3831681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22640" yWindow="7360" windowWidth="27240" windowHeight="16000" xr2:uid="{5F4F2347-5DE7-BD47-9FC5-6C8FE493BDD2}"/>
   </bookViews>
@@ -239,11 +239,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -561,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1350422-7CD6-BD43-83B7-833931238504}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,28 +573,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -922,9 +919,6 @@
       <c r="H15">
         <v>-72.754170000000002</v>
       </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>